<commit_message>
Updated excels of tanker
</commit_message>
<xml_diff>
--- a/lims_backend/tanker_arrival.xlsx
+++ b/lims_backend/tanker_arrival.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -746,6 +746,73 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>GJ2010</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Potassium Chloride</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>djcsdj</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>B101003</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>O101</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Central Admin</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>16-02-2026 17:27</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>